<commit_message>
modifications to early stem growth
</commit_message>
<xml_diff>
--- a/cbrunner/Parameters/Parameters_Disturbances.xlsx
+++ b/cbrunner/Parameters/Parameters_Disturbances.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rhember\Documents\Code_Python\fcgadgets\cbrunner\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{580D8898-9E1E-41D9-8704-328C1F3A478C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8298BE99-EBB2-4C71-BE2A-720259C86EB8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="828" yWindow="-108" windowWidth="22320" windowHeight="13176" xr2:uid="{084E029F-F488-4F82-A5F5-E3A240A0CD52}"/>
+    <workbookView xWindow="840" yWindow="-108" windowWidth="22308" windowHeight="13176" xr2:uid="{084E029F-F488-4F82-A5F5-E3A240A0CD52}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -711,10 +711,10 @@
   <dimension ref="A1:AC60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C17" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="Q2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A42" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -883,22 +883,22 @@
         <v>0</v>
       </c>
       <c r="U2" s="1">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="V2" s="1">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="W2" s="1">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="X2" s="1">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="Y2" s="1">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="Z2" s="1">
-        <v>0.95</v>
+        <v>1</v>
       </c>
       <c r="AA2" s="1">
         <f t="shared" ref="AA2:AA4" si="0">SUM(I2:L2)</f>
@@ -1212,13 +1212,13 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="1">
-        <v>0.95</v>
+        <v>0.85</v>
       </c>
       <c r="J8" s="1">
         <v>0</v>
       </c>
       <c r="K8" s="1">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="L8" s="1">
         <v>0</v>
@@ -1236,13 +1236,13 @@
         <v>0</v>
       </c>
       <c r="Q8" s="1">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="R8" s="1">
         <v>0</v>
       </c>
       <c r="S8" s="1">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="T8" s="1">
         <v>0</v>

</xml_diff>